<commit_message>
model changes and restructure
</commit_message>
<xml_diff>
--- a/data/conversations.xlsx
+++ b/data/conversations.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -567,6 +567,116 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-10-13 14:38:01</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>what is the total number of orders in july</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>8926 orders in July.</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>5b5b4eaa-0cb2-4eab-a958-dac0b2da8b2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-10-13 15:14:06</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>total number of canceled orders in july</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Total number of canceled orders in July: 257.</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0c47e2e6-2890-43fb-be0c-dfaf620e22fe</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-10-13 15:14:19</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>in august</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Sorry, we couldn't find the data you are looking for.</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0c47e2e6-2890-43fb-be0c-dfaf620e22fe</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-10-13 15:20:06</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>total number of canceled orders in july</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Sorry, we couldn't find the data you are looking for.</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0c47e2e6-2890-43fb-be0c-dfaf620e22fe</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-10-13 15:22:01</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>total number of canceled orders in july</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Total number of canceled orders in July: 257.</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0c47e2e6-2890-43fb-be0c-dfaf620e22fe</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>